<commit_message>
Adding multiplayer fix and several other changes.
</commit_message>
<xml_diff>
--- a/professions.xlsx
+++ b/professions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Zomboid\mods\DubsProfessionMod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E308AE-FF10-4EC6-B927-6728B937253C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E023E6B-AD04-4B38-8BAE-9164414BD4CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19425" yWindow="-1605" windowWidth="17190" windowHeight="17700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18555" yWindow="1845" windowWidth="17190" windowHeight="17700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DPM Balancing" sheetId="1" r:id="rId1"/>
@@ -4466,7 +4466,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
- Added Profession: "veterinarian" - Added Profession: "helicopter pilot" - Added Profession: "profession athlete basketball" - Added Profession: "professional athlete baseball" - Added Profession: "professional athlete football" - Added Profession: "professional athlete track" - Added Profession: "serial killer" - Added Profession: "tailor" - Added Profession: "landscaper"
- Fixed game traits not applying for profession's free traits
- Fixed "unlimited bad stat" infinite bug when creating character. (Note, this requires me to break immersion sadly and put in a '.' as the game uses strings to check traits, I'll see what I can do about remove it later.)

Known:
- "Football Athlete" displaying as architect, just noticed from the screenshots!
</commit_message>
<xml_diff>
--- a/professions.xlsx
+++ b/professions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Zomboid\mods\DubsProfessionMod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E023E6B-AD04-4B38-8BAE-9164414BD4CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6226A055-1D30-4783-86CB-C7BBEF6D36F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18555" yWindow="1845" windowWidth="17190" windowHeight="17700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DPM Balancing" sheetId="1" r:id="rId1"/>
@@ -991,8 +991,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BI109"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J60" sqref="J60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="V71" sqref="V71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3912,14 +3914,14 @@
       </c>
       <c r="B71">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C71">
         <v>2</v>
       </c>
       <c r="D71">
         <f t="shared" si="4"/>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="E71" t="s">
         <v>73</v>
@@ -3936,7 +3938,7 @@
         <v>-10</v>
       </c>
       <c r="J71">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L71">
         <v>5</v>
@@ -4465,7 +4467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F3C5F15-AC5C-4F40-8434-3C38AA55454A}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>

</xml_diff>